<commit_message>
excel folder been created
</commit_message>
<xml_diff>
--- a/submissions.xlsx
+++ b/submissions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="74">
   <si>
     <t>Timestamp</t>
   </si>
@@ -200,6 +200,39 @@
   </si>
   <si>
     <t>{"name":"Gogula","age":"26","sex":"Male","phone":"8008936289","email":"digitalsales@progenicslabs.com","sec-1":["Bloating or abdominal distension","Change in bowel frequency and stool form and shape"],"sec-2":["Visceral hypersensitivity","Dysregulated gut motility"],"sec-3":["Symptoms &gt; 6 months in duration","Abdominal pain &gt;1 day/week","Pain related to defecation","Type 3: Like a sausage with cracks","Type 4: Smooth, soft sausage or snake","Type 5: Soft blobs with clear-cut edges","Type 7: Watery, no solid pieces"],"sec-4":["Abdominal mass","Fecal Incontinence","Fever","Nocturnal symptoms"]}</t>
+  </si>
+  <si>
+    <t>8/9/2025, 6:15:43 pm</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>{"name":"Akhil","age":"36","sex":"Male","phone":"8008936289","email":"digitalsales@progenicslabs.com","sec-1":["Bloating or abdominal distension","Change in bowel frequency and stool form and shape"],"sec-2":["Visceral hypersensitivity","Dysregulated gut motility"],"sec-3":["Abdominal pain &gt;1 day/week","Pain related to defecation"],"sec-4":["Fecal Incontinence","Weight loss","Fever","Nocturnal symptoms"]}</t>
+  </si>
+  <si>
+    <t>8/9/2025, 6:22:44 pm</t>
+  </si>
+  <si>
+    <t>udaykiran</t>
+  </si>
+  <si>
+    <t>9966960202</t>
+  </si>
+  <si>
+    <t>gogulaudaykiran2204@gmail.com</t>
+  </si>
+  <si>
+    <t>{"name":"udaykiran","age":"23","sex":"Male","phone":"9966960202","email":"gogulaudaykiran2204@gmail.com","sec-1":["Bloating or abdominal distension","Change in bowel frequency and stool form and shape"],"sec-2":["Abnormal pain signaling","Microbiota disturbance","Gut Inflammation"],"sec-3":["Abdominal pain &gt;1 day/week","Pain related to defecation","Type 2: Lumpy and sausage-shaped","Type 5: Soft blobs with clear-cut edges","Type 7: Watery, no solid pieces"],"sec-4":["Blood in stool","Anemia or low hemoglobin","Abdominal mass","Fecal Incontinence","Nocturnal symptoms"]}</t>
+  </si>
+  <si>
+    <t>8/9/2025, 6:32:13 pm</t>
+  </si>
+  <si>
+    <t>uday kiran</t>
+  </si>
+  <si>
+    <t>{"name":"uday kiran","age":"23","sex":"Male","country-code":"+91","phone":"9966960202","email":"gogulaudaykiran2204@gmail.com","sec-1":["Recurrent abdominal pain (&gt;1 day/week in the last 3 months)","Bloating or abdominal distension","Change in bowel frequency and stool form and shape"],"sec-2":["Abnormal pain signaling","Dysregulated gut motility","Microbiota disturbance","Gut Inflammation","Dietary trigger"],"sec-3":["Symptoms &gt; 6 months in duration","Abdominal pain &gt;1 day/week","Pain related to defecation","Type 2: Lumpy and sausage-shaped","Type 4: Smooth, soft sausage or snake","Type 5: Soft blobs with clear-cut edges","Type 6: Mushy with ragged edges","Type 7: Watery, no solid pieces"],"sec-4":["Abdominal mass","Fecal Incontinence","Weight loss","Fever","Nocturnal symptoms","Family history of IBD, celiac, cancer","New symptom onset (&lt;6 months)","Recent antibiotic use","Extra-intestinal signs (rash, arthritis, eye Inflammation)"]}</t>
   </si>
 </sst>
 </file>
@@ -576,7 +609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G23"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1039,6 +1072,75 @@
         <v>62</v>
       </c>
     </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>